<commit_message>
add linear regression results table
</commit_message>
<xml_diff>
--- a/documentation/Continuous_Tbl_1_2018.xlsx
+++ b/documentation/Continuous_Tbl_1_2018.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\BRFSS\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBDF804-ED2C-4F08-8C16-C533A941866E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09970AF2-B208-446A-ACB1-180DE5A1CA28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10500" yWindow="-13695" windowWidth="23340" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17475" yWindow="-15645" windowWidth="25980" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Continuous" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Table 1 Continuous'!$A$1:$E$65</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -277,7 +280,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,14 +309,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -469,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -507,18 +502,12 @@
     <xf numFmtId="2" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -531,12 +520,6 @@
     <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -554,6 +537,31 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -901,14 +909,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.7109375" style="1" hidden="1" customWidth="1"/>
@@ -921,18 +929,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -968,19 +976,19 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17" t="str">
+      <c r="C3" s="31" t="str">
         <f>I3 &amp; ", " &amp; ROUND((J3*100), 0) &amp; "%"</f>
         <v>52984, 100%</v>
       </c>
-      <c r="D3" s="17" t="str">
+      <c r="D3" s="15" t="str">
         <f>ROUND(G3,1) &amp;", "&amp;ROUND(H3,1)</f>
         <v>7.1, 1.6</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="16" t="s">
         <v>76</v>
       </c>
       <c r="G3" s="10">
@@ -1001,21 +1009,21 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="19" t="str">
+      <c r="C4" s="32" t="str">
         <f t="shared" ref="C4:C65" si="0">I4 &amp; ", " &amp; ROUND((J4*100), 0) &amp; "%"</f>
         <v>23418, 44%</v>
       </c>
-      <c r="D4" s="19" t="str">
+      <c r="D4" s="17" t="str">
         <f t="shared" ref="D4:D65" si="1">ROUND(G4,1) &amp;", "&amp;ROUND(H4,1)</f>
         <v>7.1, 1.7</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="19">
         <v>2.257E-2</v>
       </c>
       <c r="F4" s="11"/>
@@ -1034,19 +1042,19 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="19" t="str">
+      <c r="C5" s="32" t="str">
         <f t="shared" si="0"/>
         <v>20731, 39%</v>
       </c>
-      <c r="D5" s="19" t="str">
+      <c r="D5" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7, 1.5</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11">
         <v>7.0210795427138102</v>
@@ -1063,19 +1071,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="19" t="str">
+      <c r="C6" s="32" t="str">
         <f t="shared" si="0"/>
         <v>8835, 17%</v>
       </c>
-      <c r="D6" s="19" t="str">
+      <c r="D6" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.5</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11">
         <v>7.0668930390492397</v>
@@ -1092,21 +1100,21 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="19" t="str">
+      <c r="C7" s="32" t="str">
         <f t="shared" si="0"/>
         <v>47686, 90%</v>
       </c>
-      <c r="D7" s="19" t="str">
+      <c r="D7" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.8, 1.8</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F7" s="11"/>
@@ -1125,19 +1133,19 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="19" t="str">
+      <c r="C8" s="32" t="str">
         <f t="shared" si="0"/>
         <v>5298, 10%</v>
       </c>
-      <c r="D8" s="19" t="str">
+      <c r="D8" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.6</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11">
         <v>7.0817640397600998</v>
@@ -1154,21 +1162,21 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="19" t="str">
+      <c r="C9" s="32" t="str">
         <f t="shared" si="0"/>
         <v>1090, 2%</v>
       </c>
-      <c r="D9" s="19" t="str">
+      <c r="D9" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.6, 1.6</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F9" s="11"/>
@@ -1187,19 +1195,19 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="19" t="str">
+      <c r="C10" s="32" t="str">
         <f t="shared" si="0"/>
         <v>2947, 6%</v>
       </c>
-      <c r="D10" s="19" t="str">
+      <c r="D10" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.4, 1.4</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11">
         <v>6.4356973193077698</v>
@@ -1216,19 +1224,19 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="19" t="str">
+      <c r="C11" s="32" t="str">
         <f t="shared" si="0"/>
         <v>3560, 7%</v>
       </c>
-      <c r="D11" s="19" t="str">
+      <c r="D11" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.5, 1.5</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11">
         <v>6.4918539325842701</v>
@@ -1245,19 +1253,19 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="29"/>
+      <c r="B12" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="19" t="str">
+      <c r="C12" s="32" t="str">
         <f t="shared" si="0"/>
         <v>6152, 12%</v>
       </c>
-      <c r="D12" s="19" t="str">
+      <c r="D12" s="17" t="str">
         <f>ROUND(G12,1) &amp;", "&amp;ROUND(H12,1)</f>
         <v>6.6, 1.5</v>
       </c>
-      <c r="E12" s="24"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11">
         <v>6.6311768530559201</v>
@@ -1274,19 +1282,19 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="19" t="str">
+      <c r="C13" s="32" t="str">
         <f t="shared" si="0"/>
         <v>8783, 17%</v>
       </c>
-      <c r="D13" s="19" t="str">
+      <c r="D13" s="17" t="str">
         <f t="shared" ref="D13:D14" si="3">ROUND(G13,1) &amp;", "&amp;ROUND(H13,1)</f>
         <v>6.8, 1.6</v>
       </c>
-      <c r="E13" s="24"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11">
         <v>6.8221564385745204</v>
@@ -1303,19 +1311,19 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="30"/>
+      <c r="B14" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="19" t="str">
+      <c r="C14" s="32" t="str">
         <f t="shared" si="0"/>
         <v>30452, 57%</v>
       </c>
-      <c r="D14" s="19" t="str">
+      <c r="D14" s="17" t="str">
         <f t="shared" si="3"/>
         <v>7.4, 1.5</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11">
         <v>7.3536385130697504</v>
@@ -1332,21 +1340,21 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="19" t="str">
+      <c r="C15" s="32" t="str">
         <f t="shared" si="0"/>
         <v>47805, 90%</v>
       </c>
-      <c r="D15" s="19" t="str">
+      <c r="D15" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.6</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="19">
         <v>7.0450000000000005E-4</v>
       </c>
       <c r="F15" s="11"/>
@@ -1365,19 +1373,19 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="19" t="str">
+      <c r="C16" s="32" t="str">
         <f t="shared" si="0"/>
         <v>5075, 10%</v>
       </c>
-      <c r="D16" s="19" t="str">
+      <c r="D16" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.9, 1.6</v>
       </c>
-      <c r="E16" s="25"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11">
         <v>6.8742857142857101</v>
@@ -1394,14 +1402,14 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="19" t="str">
+      <c r="A17" s="30"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>104, 0%</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11">
         <v>7.5</v>
@@ -1418,21 +1426,21 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="19" t="str">
+      <c r="C18" s="32" t="str">
         <f t="shared" ref="C18:C19" si="4">I18 &amp; ", " &amp; ROUND((J18*100), 0) &amp; "%"</f>
         <v>2233, 4%</v>
       </c>
-      <c r="D18" s="19" t="str">
+      <c r="D18" s="17" t="str">
         <f t="shared" ref="D18:D19" si="5">ROUND(G18,1) &amp;", "&amp;ROUND(H18,1)</f>
         <v>6.7, 1.8</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="19">
         <v>1.0410000000000001E-2</v>
       </c>
       <c r="F18" s="11"/>
@@ -1451,19 +1459,19 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="19" t="str">
+      <c r="C19" s="32" t="str">
         <f t="shared" si="4"/>
         <v>50162, 95%</v>
       </c>
-      <c r="D19" s="19" t="str">
+      <c r="D19" s="17" t="str">
         <f t="shared" si="5"/>
         <v>7.1, 1.6</v>
       </c>
-      <c r="E19" s="24"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11">
         <v>7.0750966867349803</v>
@@ -1480,19 +1488,19 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="19" t="str">
+      <c r="C20" s="32" t="str">
         <f t="shared" ref="C20" si="6">I20 &amp; ", " &amp; ROUND((J20*100), 0) &amp; "%"</f>
         <v>589, 1%</v>
       </c>
-      <c r="D20" s="19" t="str">
+      <c r="D20" s="17" t="str">
         <f t="shared" ref="D20" si="7">ROUND(G20,1) &amp;", "&amp;ROUND(H20,1)</f>
         <v>7, 1.7</v>
       </c>
-      <c r="E20" s="25"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11">
         <v>7.0271646859083203</v>
@@ -1509,21 +1517,21 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="19" t="str">
+      <c r="C21" s="32" t="str">
         <f t="shared" si="0"/>
         <v>43844, 83%</v>
       </c>
-      <c r="D21" s="19" t="str">
+      <c r="D21" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.5</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F21" s="11"/>
@@ -1542,19 +1550,19 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="19" t="str">
+      <c r="C22" s="32" t="str">
         <f t="shared" si="0"/>
         <v>4019, 8%</v>
       </c>
-      <c r="D22" s="19" t="str">
+      <c r="D22" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.8, 2</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11">
         <v>6.8039313262005496</v>
@@ -1571,19 +1579,19 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="19" t="str">
+      <c r="C23" s="32" t="str">
         <f t="shared" si="0"/>
         <v>1049, 2%</v>
       </c>
-      <c r="D23" s="19" t="str">
+      <c r="D23" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.7, 1.8</v>
       </c>
-      <c r="E23" s="24"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11">
         <v>6.7321258341277401</v>
@@ -1600,19 +1608,19 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="19" t="str">
+      <c r="C24" s="32" t="str">
         <f t="shared" si="0"/>
         <v>582, 1%</v>
       </c>
-      <c r="D24" s="19" t="str">
+      <c r="D24" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.5, 1.5</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11">
         <v>6.4845360824742304</v>
@@ -1629,19 +1637,19 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="19" t="str">
+      <c r="C25" s="32" t="str">
         <f t="shared" ref="C25" si="8">I25 &amp; ", " &amp; ROUND((J25*100), 0) &amp; "%"</f>
         <v>320, 1%</v>
       </c>
-      <c r="D25" s="19" t="str">
+      <c r="D25" s="17" t="str">
         <f t="shared" ref="D25" si="9">ROUND(G25,1) &amp;", "&amp;ROUND(H25,1)</f>
         <v>6.6, 1.9</v>
       </c>
-      <c r="E25" s="24"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11">
         <v>6.5968749999999998</v>
@@ -1658,19 +1666,19 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="29"/>
+      <c r="B26" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="19" t="str">
+      <c r="C26" s="32" t="str">
         <f t="shared" ref="C26:C27" si="10">I26 &amp; ", " &amp; ROUND((J26*100), 0) &amp; "%"</f>
         <v>2162, 4%</v>
       </c>
-      <c r="D26" s="19" t="str">
+      <c r="D26" s="17" t="str">
         <f t="shared" ref="D26:D27" si="11">ROUND(G26,1) &amp;", "&amp;ROUND(H26,1)</f>
         <v>6.8, 2</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="20"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11">
         <v>6.7641073080481</v>
@@ -1687,19 +1695,19 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13" t="s">
+      <c r="A27" s="30"/>
+      <c r="B27" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="19" t="str">
+      <c r="C27" s="32" t="str">
         <f t="shared" si="10"/>
         <v>1008, 2%</v>
       </c>
-      <c r="D27" s="19" t="str">
+      <c r="D27" s="17" t="str">
         <f t="shared" si="11"/>
         <v>7.1, 1.7</v>
       </c>
-      <c r="E27" s="25"/>
+      <c r="E27" s="21"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11">
         <v>7.0545634920634903</v>
@@ -1716,21 +1724,21 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="19" t="str">
+      <c r="C28" s="32" t="str">
         <f t="shared" ref="C28:C31" si="12">I28 &amp; ", " &amp; ROUND((J28*100), 0) &amp; "%"</f>
         <v>36076, 68%</v>
       </c>
-      <c r="D28" s="19" t="str">
+      <c r="D28" s="17" t="str">
         <f t="shared" ref="D28:D31" si="13">ROUND(G28,1) &amp;", "&amp;ROUND(H28,1)</f>
         <v>7.1, 1.5</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F28" s="11"/>
@@ -1749,19 +1757,19 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="19" t="str">
+      <c r="C29" s="32" t="str">
         <f t="shared" si="12"/>
         <v>14741, 28%</v>
       </c>
-      <c r="D29" s="19" t="str">
+      <c r="D29" s="17" t="str">
         <f t="shared" si="13"/>
         <v>7.1, 1.8</v>
       </c>
-      <c r="E29" s="24"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11">
         <v>7.0723153110372401</v>
@@ -1778,19 +1786,19 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="19" t="str">
+      <c r="C30" s="32" t="str">
         <f t="shared" si="12"/>
         <v>941, 2%</v>
       </c>
-      <c r="D30" s="19" t="str">
+      <c r="D30" s="17" t="str">
         <f t="shared" si="13"/>
         <v>6.8, 2</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="20"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11">
         <v>6.7917109458023397</v>
@@ -1807,19 +1815,19 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13" t="s">
+      <c r="A31" s="30"/>
+      <c r="B31" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="19" t="str">
+      <c r="C31" s="32" t="str">
         <f t="shared" si="12"/>
         <v>1226, 2%</v>
       </c>
-      <c r="D31" s="19" t="str">
+      <c r="D31" s="17" t="str">
         <f t="shared" si="13"/>
         <v>6.8, 1.7</v>
       </c>
-      <c r="E31" s="25"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11">
         <v>6.8401305057096202</v>
@@ -1835,22 +1843,22 @@
         <v>2.3139060848558057E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="17" t="str">
+      <c r="C32" s="31" t="str">
         <f t="shared" si="0"/>
         <v>1908, 4%</v>
       </c>
-      <c r="D32" s="17" t="str">
+      <c r="D32" s="15" t="str">
         <f t="shared" si="1"/>
         <v>7.2, 2.2</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="22">
         <v>0.13950000000000001</v>
       </c>
       <c r="G32" s="10">
@@ -1868,19 +1876,19 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16" t="s">
+      <c r="A33" s="29"/>
+      <c r="B33" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="17" t="str">
+      <c r="C33" s="31" t="str">
         <f t="shared" ref="C33" si="14">I33 &amp; ", " &amp; ROUND((J33*100), 0) &amp; "%"</f>
         <v>14025, 26%</v>
       </c>
-      <c r="D33" s="17" t="str">
+      <c r="D33" s="15" t="str">
         <f t="shared" ref="D33" si="15">ROUND(G33,1) &amp;", "&amp;ROUND(H33,1)</f>
         <v>7.1, 1.7</v>
       </c>
-      <c r="E33" s="27"/>
+      <c r="E33" s="23"/>
       <c r="G33" s="10">
         <v>7.07871657754011</v>
       </c>
@@ -1896,19 +1904,19 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16" t="s">
+      <c r="A34" s="29"/>
+      <c r="B34" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="17" t="str">
+      <c r="C34" s="31" t="str">
         <f t="shared" si="0"/>
         <v>16603, 31%</v>
       </c>
-      <c r="D34" s="17" t="str">
+      <c r="D34" s="15" t="str">
         <f t="shared" si="1"/>
         <v>7, 1.6</v>
       </c>
-      <c r="E34" s="27"/>
+      <c r="E34" s="23"/>
       <c r="G34" s="10">
         <v>6.9612720592663999</v>
       </c>
@@ -1924,19 +1932,19 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16" t="s">
+      <c r="A35" s="29"/>
+      <c r="B35" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="17" t="str">
+      <c r="C35" s="31" t="str">
         <f t="shared" si="0"/>
         <v>20339, 38%</v>
       </c>
-      <c r="D35" s="17" t="str">
+      <c r="D35" s="15" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.4</v>
       </c>
-      <c r="E35" s="27"/>
+      <c r="E35" s="23"/>
       <c r="G35" s="10">
         <v>7.1123457397118797</v>
       </c>
@@ -1952,19 +1960,19 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16" t="s">
+      <c r="A36" s="30"/>
+      <c r="B36" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="17" t="str">
+      <c r="C36" s="31" t="str">
         <f t="shared" ref="C36" si="16">I36 &amp; ", " &amp; ROUND((J36*100), 0) &amp; "%"</f>
         <v>109, 0%</v>
       </c>
-      <c r="D36" s="17" t="str">
+      <c r="D36" s="15" t="str">
         <f t="shared" ref="D36" si="17">ROUND(G36,1) &amp;", "&amp;ROUND(H36,1)</f>
         <v>7.2, 1.8</v>
       </c>
-      <c r="E36" s="28"/>
+      <c r="E36" s="24"/>
       <c r="G36" s="10">
         <v>7.1743119266055002</v>
       </c>
@@ -1979,22 +1987,22 @@
         <v>2.0572248225879512E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="19" t="str">
+      <c r="C37" s="33" t="str">
         <f t="shared" ref="C37:C45" si="18">I37 &amp; ", " &amp; ROUND((J37*100), 0) &amp; "%"</f>
         <v>920, 2%</v>
       </c>
-      <c r="D37" s="19" t="str">
+      <c r="D37" s="17" t="str">
         <f t="shared" ref="D37:D45" si="19">ROUND(G37,1) &amp;", "&amp;ROUND(H37,1)</f>
         <v>6.7, 2.2</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="19">
         <v>2.5270000000000002E-4</v>
       </c>
       <c r="F37" s="11"/>
@@ -2013,19 +2021,19 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13" t="s">
+      <c r="A38" s="29"/>
+      <c r="B38" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="19" t="str">
+      <c r="C38" s="33" t="str">
         <f t="shared" si="18"/>
         <v>1720, 3%</v>
       </c>
-      <c r="D38" s="19" t="str">
+      <c r="D38" s="17" t="str">
         <f t="shared" si="19"/>
         <v>7, 2.2</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11">
         <v>7.0325581395348804</v>
@@ -2042,19 +2050,19 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13" t="s">
+      <c r="A39" s="29"/>
+      <c r="B39" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="19" t="str">
+      <c r="C39" s="33" t="str">
         <f t="shared" si="18"/>
         <v>2411, 5%</v>
       </c>
-      <c r="D39" s="19" t="str">
+      <c r="D39" s="17" t="str">
         <f t="shared" si="19"/>
         <v>7, 2</v>
       </c>
-      <c r="E39" s="24"/>
+      <c r="E39" s="20"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11">
         <v>7.0103691414350902</v>
@@ -2071,19 +2079,19 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="19" t="str">
+      <c r="C40" s="33" t="str">
         <f t="shared" si="18"/>
         <v>3776, 7%</v>
       </c>
-      <c r="D40" s="19" t="str">
+      <c r="D40" s="17" t="str">
         <f t="shared" si="19"/>
         <v>7, 1.8</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="20"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11">
         <v>7.04872881355932</v>
@@ -2100,19 +2108,19 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13" t="s">
+      <c r="A41" s="29"/>
+      <c r="B41" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="19" t="str">
+      <c r="C41" s="33" t="str">
         <f t="shared" si="18"/>
         <v>5258, 10%</v>
       </c>
-      <c r="D41" s="19" t="str">
+      <c r="D41" s="17" t="str">
         <f t="shared" si="19"/>
         <v>7.1, 1.7</v>
       </c>
-      <c r="E41" s="24"/>
+      <c r="E41" s="20"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11">
         <v>7.1340813997717802</v>
@@ -2129,19 +2137,19 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13" t="s">
+      <c r="A42" s="29"/>
+      <c r="B42" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="19" t="str">
+      <c r="C42" s="33" t="str">
         <f t="shared" si="18"/>
         <v>7560, 14%</v>
       </c>
-      <c r="D42" s="19" t="str">
+      <c r="D42" s="17" t="str">
         <f t="shared" si="19"/>
         <v>7.1, 1.6</v>
       </c>
-      <c r="E42" s="24"/>
+      <c r="E42" s="20"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11">
         <v>7.08875661375661</v>
@@ -2158,19 +2166,19 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13" t="s">
+      <c r="A43" s="29"/>
+      <c r="B43" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C43" s="19" t="str">
+      <c r="C43" s="33" t="str">
         <f t="shared" si="18"/>
         <v>8824, 17%</v>
       </c>
-      <c r="D43" s="19" t="str">
+      <c r="D43" s="17" t="str">
         <f t="shared" si="19"/>
         <v>7.1, 1.4</v>
       </c>
-      <c r="E43" s="24"/>
+      <c r="E43" s="20"/>
       <c r="F43" s="11"/>
       <c r="G43" s="11">
         <v>7.0538304623753403</v>
@@ -2187,19 +2195,19 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13" t="s">
+      <c r="A44" s="29"/>
+      <c r="B44" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="19" t="str">
+      <c r="C44" s="33" t="str">
         <f t="shared" si="18"/>
         <v>15935, 30%</v>
       </c>
-      <c r="D44" s="19" t="str">
+      <c r="D44" s="17" t="str">
         <f t="shared" si="19"/>
         <v>7, 1.3</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="20"/>
       <c r="F44" s="11"/>
       <c r="G44" s="11">
         <v>7.0128020081581397</v>
@@ -2216,19 +2224,19 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13" t="s">
+      <c r="A45" s="30"/>
+      <c r="B45" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="19" t="str">
+      <c r="C45" s="33" t="str">
         <f t="shared" si="18"/>
         <v>6576, 12%</v>
       </c>
-      <c r="D45" s="19" t="str">
+      <c r="D45" s="17" t="str">
         <f t="shared" si="19"/>
         <v>7.2, 1.7</v>
       </c>
-      <c r="E45" s="25"/>
+      <c r="E45" s="21"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11">
         <v>7.1630170316301696</v>
@@ -2245,21 +2253,21 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="19" t="str">
+      <c r="C46" s="33" t="str">
         <f t="shared" si="0"/>
         <v>475, 1%</v>
       </c>
-      <c r="D46" s="19" t="str">
+      <c r="D46" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 2.2</v>
       </c>
-      <c r="E46" s="23" t="s">
+      <c r="E46" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F46" s="11"/>
@@ -2278,19 +2286,19 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13" t="s">
+      <c r="A47" s="29"/>
+      <c r="B47" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="19" t="str">
+      <c r="C47" s="33" t="str">
         <f t="shared" si="0"/>
         <v>12493, 24%</v>
       </c>
-      <c r="D47" s="19" t="str">
+      <c r="D47" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.2, 1.6</v>
       </c>
-      <c r="E47" s="24"/>
+      <c r="E47" s="20"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11">
         <v>7.1696149843912602</v>
@@ -2307,19 +2315,19 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13" t="s">
+      <c r="A48" s="29"/>
+      <c r="B48" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="19" t="str">
+      <c r="C48" s="33" t="str">
         <f t="shared" si="0"/>
         <v>22206, 42%</v>
       </c>
-      <c r="D48" s="19" t="str">
+      <c r="D48" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.5</v>
       </c>
-      <c r="E48" s="24"/>
+      <c r="E48" s="20"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11">
         <v>7.0750698009547</v>
@@ -2336,19 +2344,19 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13" t="s">
+      <c r="A49" s="29"/>
+      <c r="B49" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="19" t="str">
+      <c r="C49" s="33" t="str">
         <f t="shared" si="0"/>
         <v>16669, 31%</v>
       </c>
-      <c r="D49" s="19" t="str">
+      <c r="D49" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7, 1.6</v>
       </c>
-      <c r="E49" s="24"/>
+      <c r="E49" s="20"/>
       <c r="F49" s="11"/>
       <c r="G49" s="11">
         <v>6.95866578678985</v>
@@ -2365,19 +2373,19 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13" t="s">
+      <c r="A50" s="30"/>
+      <c r="B50" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="19" t="str">
+      <c r="C50" s="33" t="str">
         <f t="shared" si="0"/>
         <v>1141, 2%</v>
       </c>
-      <c r="D50" s="19" t="str">
+      <c r="D50" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.9, 1.8</v>
       </c>
-      <c r="E50" s="25"/>
+      <c r="E50" s="21"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11">
         <v>6.9184925503943902</v>
@@ -2394,21 +2402,21 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="19" t="str">
+      <c r="C51" s="33" t="str">
         <f t="shared" si="0"/>
         <v>7854, 15%</v>
       </c>
-      <c r="D51" s="19" t="str">
+      <c r="D51" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.7, 1.8</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F51" s="11"/>
@@ -2427,19 +2435,19 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13" t="s">
+      <c r="A52" s="29"/>
+      <c r="B52" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="19" t="str">
+      <c r="C52" s="33" t="str">
         <f t="shared" si="0"/>
         <v>44820, 85%</v>
       </c>
-      <c r="D52" s="19" t="str">
+      <c r="D52" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.5</v>
       </c>
-      <c r="E52" s="24"/>
+      <c r="E52" s="20"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11">
         <v>7.11755912539045</v>
@@ -2456,19 +2464,19 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13" t="s">
+      <c r="A53" s="30"/>
+      <c r="B53" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="19" t="str">
+      <c r="C53" s="33" t="str">
         <f t="shared" si="0"/>
         <v>310, 1%</v>
       </c>
-      <c r="D53" s="19" t="str">
+      <c r="D53" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.5</v>
       </c>
-      <c r="E53" s="25"/>
+      <c r="E53" s="21"/>
       <c r="F53" s="11"/>
       <c r="G53" s="11">
         <v>7.1193548387096799</v>
@@ -2485,21 +2493,21 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="17" t="str">
+      <c r="C54" s="31" t="str">
         <f t="shared" si="0"/>
         <v>39839, 75%</v>
       </c>
-      <c r="D54" s="17" t="str">
+      <c r="D54" s="15" t="str">
         <f t="shared" si="1"/>
         <v>7, 1.5</v>
       </c>
-      <c r="E54" s="26">
+      <c r="E54" s="22">
         <v>0.11899999999999999</v>
       </c>
       <c r="G54" s="10">
@@ -2517,19 +2525,19 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16" t="s">
+      <c r="A55" s="29"/>
+      <c r="B55" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="17" t="str">
+      <c r="C55" s="31" t="str">
         <f t="shared" si="0"/>
         <v>13062, 25%</v>
       </c>
-      <c r="D55" s="17" t="str">
+      <c r="D55" s="15" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.9</v>
       </c>
-      <c r="E55" s="27"/>
+      <c r="E55" s="23"/>
       <c r="G55" s="10">
         <v>7.1231817485836801</v>
       </c>
@@ -2545,19 +2553,19 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16" t="s">
+      <c r="A56" s="30"/>
+      <c r="B56" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="17" t="str">
+      <c r="C56" s="31" t="str">
         <f t="shared" si="0"/>
         <v>83, 0%</v>
       </c>
-      <c r="D56" s="17" t="str">
+      <c r="D56" s="15" t="str">
         <f t="shared" si="1"/>
         <v>7.2, 2.4</v>
       </c>
-      <c r="E56" s="28"/>
+      <c r="E56" s="24"/>
       <c r="G56" s="10">
         <v>7.2168674698795199</v>
       </c>
@@ -2573,21 +2581,21 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="19" t="str">
+      <c r="C57" s="33" t="str">
         <f t="shared" ref="C57:C59" si="20">I57 &amp; ", " &amp; ROUND((J57*100), 0) &amp; "%"</f>
         <v>50609, 96%</v>
       </c>
-      <c r="D57" s="19" t="str">
+      <c r="D57" s="17" t="str">
         <f t="shared" ref="D57:D59" si="21">ROUND(G57,1) &amp;", "&amp;ROUND(H57,1)</f>
         <v>7.1, 1.6</v>
       </c>
-      <c r="E57" s="23">
+      <c r="E57" s="19">
         <v>1.0039999999999999E-3</v>
       </c>
       <c r="F57" s="11"/>
@@ -2606,19 +2614,19 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13" t="s">
+      <c r="A58" s="29"/>
+      <c r="B58" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="19" t="str">
+      <c r="C58" s="33" t="str">
         <f t="shared" si="20"/>
         <v>2218, 4%</v>
       </c>
-      <c r="D58" s="19" t="str">
+      <c r="D58" s="17" t="str">
         <f t="shared" si="21"/>
         <v>6.8, 1.9</v>
       </c>
-      <c r="E58" s="24"/>
+      <c r="E58" s="20"/>
       <c r="F58" s="11"/>
       <c r="G58" s="11">
         <v>6.7971145175834096</v>
@@ -2635,19 +2643,19 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13" t="s">
+      <c r="A59" s="30"/>
+      <c r="B59" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="19" t="str">
+      <c r="C59" s="33" t="str">
         <f t="shared" si="20"/>
         <v>157, 0%</v>
       </c>
-      <c r="D59" s="19" t="str">
+      <c r="D59" s="17" t="str">
         <f t="shared" si="21"/>
         <v>7.1, 2</v>
       </c>
-      <c r="E59" s="25"/>
+      <c r="E59" s="21"/>
       <c r="F59" s="11"/>
       <c r="G59" s="11">
         <v>7.0636942675159204</v>
@@ -2664,21 +2672,21 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="19" t="str">
+      <c r="C60" s="33" t="str">
         <f t="shared" si="0"/>
         <v>7850, 15%</v>
       </c>
-      <c r="D60" s="19" t="str">
+      <c r="D60" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.4</v>
       </c>
-      <c r="E60" s="23" t="s">
+      <c r="E60" s="19" t="s">
         <v>77</v>
       </c>
       <c r="F60" s="11"/>
@@ -2697,19 +2705,19 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13" t="s">
+      <c r="A61" s="29"/>
+      <c r="B61" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C61" s="19" t="str">
+      <c r="C61" s="33" t="str">
         <f t="shared" si="0"/>
         <v>16288, 31%</v>
       </c>
-      <c r="D61" s="19" t="str">
+      <c r="D61" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.3</v>
       </c>
-      <c r="E61" s="24"/>
+      <c r="E61" s="20"/>
       <c r="F61" s="11"/>
       <c r="G61" s="11">
         <v>7.1079936149312397</v>
@@ -2726,19 +2734,19 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13" t="s">
+      <c r="A62" s="29"/>
+      <c r="B62" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C62" s="19" t="str">
+      <c r="C62" s="33" t="str">
         <f t="shared" si="0"/>
         <v>17561, 33%</v>
       </c>
-      <c r="D62" s="19" t="str">
+      <c r="D62" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.1, 1.5</v>
       </c>
-      <c r="E62" s="24"/>
+      <c r="E62" s="20"/>
       <c r="F62" s="11"/>
       <c r="G62" s="11">
         <v>7.0646318546779803</v>
@@ -2755,19 +2763,19 @@
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13" t="s">
+      <c r="A63" s="29"/>
+      <c r="B63" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="19" t="str">
+      <c r="C63" s="33" t="str">
         <f t="shared" si="0"/>
         <v>7943, 15%</v>
       </c>
-      <c r="D63" s="19" t="str">
+      <c r="D63" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7, 1.9</v>
       </c>
-      <c r="E63" s="24"/>
+      <c r="E63" s="20"/>
       <c r="F63" s="11"/>
       <c r="G63" s="11">
         <v>6.9605942339166598</v>
@@ -2784,19 +2792,19 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13" t="s">
+      <c r="A64" s="29"/>
+      <c r="B64" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C64" s="19" t="str">
+      <c r="C64" s="33" t="str">
         <f t="shared" si="0"/>
         <v>3207, 6%</v>
       </c>
-      <c r="D64" s="19" t="str">
+      <c r="D64" s="17" t="str">
         <f t="shared" si="1"/>
         <v>6.9, 2.5</v>
       </c>
-      <c r="E64" s="24"/>
+      <c r="E64" s="20"/>
       <c r="F64" s="11"/>
       <c r="G64" s="11">
         <v>6.9298409728718404</v>
@@ -2813,19 +2821,19 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13" t="s">
+      <c r="A65" s="30"/>
+      <c r="B65" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="19" t="str">
+      <c r="C65" s="33" t="str">
         <f t="shared" si="0"/>
         <v>135, 0%</v>
       </c>
-      <c r="D65" s="19" t="str">
+      <c r="D65" s="17" t="str">
         <f t="shared" si="1"/>
         <v>7.2, 2</v>
       </c>
-      <c r="E65" s="25"/>
+      <c r="E65" s="21"/>
       <c r="F65" s="11"/>
       <c r="G65" s="11">
         <v>7.1555555555555603</v>
@@ -2842,12 +2850,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="E60:E65"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="E46:E50"/>
+  <mergeCells count="29">
+    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A45"/>
+    <mergeCell ref="A46:A50"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="E37:E45"/>
     <mergeCell ref="E32:E36"/>
@@ -2858,8 +2870,18 @@
     <mergeCell ref="E9:E14"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E18:E20"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="E60:E65"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E46:E50"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="68" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup scale="70" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>